<commit_message>
Updated schedule page to use a JavaScript calendar.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox/School/Teaching/course_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7A71D-415A-A644-BA45-93B685E593C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4729D03-AD8F-B94B-8A17-32171B14A960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="6600" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="2660" yWindow="9360" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -68,27 +68,6 @@
     <t>9:00 pm</t>
   </si>
   <si>
-    <t>8:30pm</t>
-  </si>
-  <si>
-    <t>[Chapter 1](/chapters/chapter1)</t>
-  </si>
-  <si>
-    <t>[Chapter 2](/chapters/chapter2)</t>
-  </si>
-  <si>
-    <t>[Chapter 3](/chapters/chapter3)</t>
-  </si>
-  <si>
-    <t>[Final Exam](/assignments/exams/)</t>
-  </si>
-  <si>
-    <t>[Chapter 4](/chapters/chapter4)</t>
-  </si>
-  <si>
-    <t>[Chapter 5](/chapters/chapter5)</t>
-  </si>
-  <si>
     <t>Week 6</t>
   </si>
   <si>
@@ -125,25 +104,85 @@
     <t>President's Day</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
     <t>NO CLASS - Spring Recess</t>
   </si>
   <si>
-    <t>Week 15</t>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>/chapters/chapter1</t>
+  </si>
+  <si>
+    <t>/chapters/chapter2</t>
+  </si>
+  <si>
+    <t>/chapters/chapter3</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Chapter 2</t>
+  </si>
+  <si>
+    <t>Chapter 3</t>
+  </si>
+  <si>
+    <t>Chapter 4</t>
+  </si>
+  <si>
+    <t>Chapter 5</t>
+  </si>
+  <si>
+    <t>/assignments/exams/</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Week 1 Meetup</t>
+  </si>
+  <si>
+    <t>Week 2 Meetup</t>
+  </si>
+  <si>
+    <t>Week 3 Meetup</t>
+  </si>
+  <si>
+    <t>Week 4 Meetup</t>
+  </si>
+  <si>
+    <t>Week 5 Meetup</t>
+  </si>
+  <si>
+    <t>Week 6 Meetup</t>
+  </si>
+  <si>
+    <t>Week 7 Meetup</t>
+  </si>
+  <si>
+    <t>Week 8 Meetup</t>
+  </si>
+  <si>
+    <t>Week 9 Meetup</t>
+  </si>
+  <si>
+    <t>Week 10 Meetup</t>
+  </si>
+  <si>
+    <t>Week 11 Meetup</t>
+  </si>
+  <si>
+    <t>Week 12 Meetup</t>
+  </si>
+  <si>
+    <t>Week 13 Meetup</t>
+  </si>
+  <si>
+    <t>Week 14 Meetup</t>
+  </si>
+  <si>
+    <t>Week 15 Meetup</t>
   </si>
 </sst>
 </file>
@@ -518,7 +557,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -571,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -585,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -599,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -613,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -627,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -641,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -655,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -663,7 +702,7 @@
         <v>44286</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -677,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -691,7 +730,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -705,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -719,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -733,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,7 +786,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -755,13 +794,13 @@
         <v>44335</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -772,19 +811,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD67FB80-52EB-7F41-88A6-58F30ED23B0C}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -794,8 +833,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44225</v>
       </c>
@@ -803,21 +845,27 @@
         <v>44234</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43869</v>
+        <v>44235</v>
       </c>
       <c r="B3" s="2">
         <v>44241</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44242</v>
       </c>
@@ -825,10 +873,10 @@
         <v>44242</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44242</v>
       </c>
@@ -836,10 +884,13 @@
         <v>44248</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44249</v>
       </c>
@@ -847,10 +898,10 @@
         <v>44255</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44256</v>
       </c>
@@ -858,10 +909,10 @@
         <v>44262</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44263</v>
       </c>
@@ -869,10 +920,10 @@
         <v>44269</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44270</v>
       </c>
@@ -880,21 +931,21 @@
         <v>44276</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44277</v>
       </c>
       <c r="B10" s="2">
-        <v>46109</v>
+        <v>44283</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44282</v>
       </c>
@@ -902,10 +953,10 @@
         <v>44290</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44291</v>
       </c>
@@ -913,10 +964,10 @@
         <v>44297</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44298</v>
       </c>
@@ -924,10 +975,10 @@
         <v>44304</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44305</v>
       </c>
@@ -935,10 +986,10 @@
         <v>44311</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44312</v>
       </c>
@@ -946,10 +997,10 @@
         <v>44318</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44319</v>
       </c>
@@ -957,10 +1008,10 @@
         <v>44325</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44326</v>
       </c>
@@ -968,10 +1019,10 @@
         <v>44333</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44334</v>
       </c>
@@ -979,10 +1030,10 @@
         <v>44334</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44335</v>
       </c>
@@ -990,7 +1041,10 @@
         <v>44341</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>